<commit_message>
feat: :sparkles: get by cf
</commit_message>
<xml_diff>
--- a/resumes.xlsx
+++ b/resumes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G151"/>
+  <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,6 +466,11 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>job_name</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>skills</t>
         </is>
       </c>
@@ -491,7 +496,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Dưới 1 năm</t>
+          <t>3 năm</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -501,7 +506,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>PHP, Git, VueJS</t>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Kotlin, Flutter, React Native, Swift, iOS</t>
         </is>
       </c>
     </row>
@@ -536,7 +546,12 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Kiểm thử chấp nhận người dùng (User acceptance testing), Kiểm thử tích hợp (Integration testing), Kiểm thử giao diện người dùng (User interface testing), Kiểm thử tự động (Automation testing), Kiểm thử hồi quy (Regression testing)</t>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Ruby, MongoDB, .NET, VueJS, Git</t>
         </is>
       </c>
     </row>
@@ -561,7 +576,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Dưới 1 năm</t>
+          <t>4 năm</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -571,7 +586,12 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Objective-C, iOS, React Native</t>
+          <t>Tester/ QA/ QC</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Kiểm thử tự động (Automation testing), Báo cáo kiểm thử (Test report), Kiểm thử hệ thống (System testing), Kiểm thử tích hợp (Integration testing), Kiểm thử chấp nhận người dùng (User acceptance testing), Kiểm thử giao diện người dùng (User interface testing)</t>
         </is>
       </c>
     </row>
@@ -596,7 +616,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Dưới 1 năm</t>
+          <t>4 năm</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -606,7 +626,12 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Kiểm thử chức năng (Functional testing), Kiểm thử bảo mật (Security testing), Kiểm thử hiệu năng (Performance testing)</t>
+          <t>Mobile Developer</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Đặc tả kiểm thử (Test case specification), Kiểm thử tích hợp (Integration testing), Báo cáo kiểm thử (Test report), Kiểm thử bảo mật (Security testing), Kiểm thử tự động (Automation testing)</t>
         </is>
       </c>
     </row>
@@ -631,7 +656,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Dưới 1 năm</t>
+          <t>3 năm</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -641,7 +666,12 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Kiểm thử chức năng (Functional testing), Kiểm thử tự động (Automation testing), Kiểm thử đơn vị (Unit testing)</t>
+          <t>Mobile Developer</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Kiểm thử đơn vị (Unit testing), Kiểm thử chấp nhận người dùng (User acceptance testing), Kiểm thử bảo mật (Security testing), Kiểm thử tự động (Automation testing), Báo cáo kiểm thử (Test report)</t>
         </is>
       </c>
     </row>
@@ -676,7 +706,12 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>React Native, Swift, Android, Objective-C</t>
+          <t>Mobile Developer</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Objective-C, Kotlin, Flutter, iOS, Swift</t>
         </is>
       </c>
     </row>
@@ -701,7 +736,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Dưới 1 năm</t>
+          <t>2 năm</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -711,7 +746,12 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Android, iOS, Kotlin</t>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Git, Laravel, Ruby, PostgreSQL, PHP</t>
         </is>
       </c>
     </row>
@@ -736,7 +776,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Dưới 1 năm</t>
+          <t>4 năm</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -746,7 +786,12 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Objective-C, Kotlin, Flutter</t>
+          <t>Mobile Developer</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Đặc tả kiểm thử (Test case specification), Phân tích yêu cầu (Requirement analysis), Kiểm thử tự động (Automation testing), Kiểm thử hiệu năng (Performance testing), Kiểm thử chức năng (Functional testing), Kiểm thử tải (Load testing)</t>
         </is>
       </c>
     </row>
@@ -771,7 +816,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>3 năm</t>
+          <t>2 năm</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -781,7 +826,12 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>AngularJS, Git, VueJS, MongoDB, BackEnd, Python, Ruby on Rails</t>
+          <t>Tester/ QA/ QC</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Kiểm thử tự động (Automation testing), Kiểm thử chức năng (Functional testing), Kiểm thử hiệu năng (Performance testing), Kiểm thử chấp nhận người dùng (User acceptance testing), Đặc tả kiểm thử (Test case specification)</t>
         </is>
       </c>
     </row>
@@ -806,7 +856,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1 năm</t>
+          <t>2 năm</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -816,7 +866,12 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>iOS, Android, React Native, Swift, Flutter</t>
+          <t>Tester/ QA/ QC</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>FrontEnd, BackEnd, NodeJS, Java, Spring Framework</t>
         </is>
       </c>
     </row>
@@ -851,7 +906,12 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>PHP, FrontEnd, PostgreSQL, JavaScript, Bootstrap, Sass/Less, Java</t>
+          <t>Tester/ QA/ QC</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Objective-C, Swift, React Native, iOS, Kotlin</t>
         </is>
       </c>
     </row>
@@ -876,7 +936,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>1 năm</t>
+          <t>4 năm</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -886,7 +946,12 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Báo cáo kiểm thử (Test report), Kiểm thử tích hợp (Integration testing), Kiểm thử hồi quy (Regression testing), Đặc tả kiểm thử (Test case specification)</t>
+          <t>Mobile Developer</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Kotlin, Objective-C, React Native, Swift, Flutter, iOS, Android</t>
         </is>
       </c>
     </row>
@@ -921,7 +986,12 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Kiểm thử chức năng (Functional testing), Đặc tả kiểm thử (Test case specification), Kiểm thử tải (Load testing), Kiểm thử chấp nhận người dùng (User acceptance testing), Kiểm thử tích hợp (Integration testing), Phân tích yêu cầu (Requirement analysis), Kiểm thử giao diện người dùng (User interface testing)</t>
+          <t>Tester/ QA/ QC</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Flutter, React Native, Swift, Kotlin, iOS, Objective-C, Android</t>
         </is>
       </c>
     </row>
@@ -956,7 +1026,12 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Flutter, Android, Objective-C, Swift, Kotlin</t>
+          <t>Mobile Developer</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>PostgreSQL, Java, Laravel, Ruby</t>
         </is>
       </c>
     </row>
@@ -981,7 +1056,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>3 năm</t>
+          <t>2 năm</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -991,7 +1066,12 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Android, iOS, Swift, Objective-C, Kotlin, React Native, Flutter</t>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>BackEnd, Material UI, Django, JavaScript, Python</t>
         </is>
       </c>
     </row>
@@ -1016,7 +1096,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Dưới 1 năm</t>
+          <t>4 năm</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1026,7 +1106,12 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Objective-C, Android, React Native</t>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Kiểm thử đơn vị (Unit testing), Báo cáo kiểm thử (Test report), Kiểm thử tích hợp (Integration testing), Kiểm thử hiệu năng (Performance testing), Kiểm thử giao diện người dùng (User interface testing)</t>
         </is>
       </c>
     </row>
@@ -1061,7 +1146,12 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Kiểm thử bảo mật (Security testing), Kiểm thử hệ thống (System testing), Kiểm thử chức năng (Functional testing), Kiểm thử tự động (Automation testing)</t>
+          <t>Tester/ QA/ QC</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Kiểm thử hiệu năng (Performance testing), Kiểm thử bảo mật (Security testing), Kiểm thử hồi quy (Regression testing), Kiểm thử đơn vị (Unit testing)</t>
         </is>
       </c>
     </row>
@@ -1086,7 +1176,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1 năm</t>
+          <t>2 năm</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1096,7 +1186,12 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>PHP, Java, FrontEnd, NodeJS</t>
+          <t>Mobile Developer</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>iOS, Swift, Objective-C, React Native, Kotlin</t>
         </is>
       </c>
     </row>
@@ -1121,7 +1216,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1 năm</t>
+          <t>4 năm</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1131,7 +1226,12 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Spring Framework, JavaScript, FrontEnd, Laravel</t>
+          <t>Mobile Developer</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Flutter, Swift, Kotlin, Objective-C, iOS, Android, React Native</t>
         </is>
       </c>
     </row>
@@ -1156,7 +1256,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1 năm</t>
+          <t>3 năm</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1166,7 +1266,12 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>PostgreSQL, FrontEnd, PHP, Git, Django</t>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Kiểm thử tải (Load testing), Phân tích yêu cầu (Requirement analysis), Kiểm thử tích hợp (Integration testing), Kiểm thử hiệu năng (Performance testing), Kiểm thử hồi quy (Regression testing), Báo cáo kiểm thử (Test report), Kiểm thử đơn vị (Unit testing)</t>
         </is>
       </c>
     </row>
@@ -1201,7 +1306,12 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Flask, Django, ReactJS, JavaScript</t>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Đặc tả kiểm thử (Test case specification), Kiểm thử chức năng (Functional testing), Báo cáo kiểm thử (Test report), Kiểm thử bảo mật (Security testing), Kiểm thử đơn vị (Unit testing)</t>
         </is>
       </c>
     </row>
@@ -1226,7 +1336,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1 năm</t>
+          <t>3 năm</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1236,7 +1346,12 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Kiểm thử tải (Load testing), Kiểm thử hồi quy (Regression testing), Kiểm thử chấp nhận người dùng (User acceptance testing), Kiểm thử đơn vị (Unit testing)</t>
+          <t>Tester/ QA/ QC</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Kiểm thử giao diện người dùng (User interface testing), Kiểm thử bảo mật (Security testing), Kiểm thử tải (Load testing), Báo cáo kiểm thử (Test report), Kiểm thử chức năng (Functional testing), Đặc tả kiểm thử (Test case specification), Kiểm thử đơn vị (Unit testing)</t>
         </is>
       </c>
     </row>
@@ -1271,7 +1386,12 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Spring Framework, PostgreSQL, NodeJS, AngularJS, PHP</t>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>ReactJS, jQuery, Git, VueJS, Ruby</t>
         </is>
       </c>
     </row>
@@ -1296,7 +1416,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2 năm</t>
+          <t>1 năm</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1306,7 +1426,12 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>TypeScript, jQuery, Spring Framework, Ruby on Rails, PHP</t>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Đặc tả kiểm thử (Test case specification), Kiểm thử bảo mật (Security testing), Kiểm thử chức năng (Functional testing), Báo cáo kiểm thử (Test report), Kiểm thử đơn vị (Unit testing)</t>
         </is>
       </c>
     </row>
@@ -1341,7 +1466,12 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Kotlin, iOS, React Native, Android, Swift, Flutter</t>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>NestJS, TypeScript, Ruby, Sass/Less, BackEnd, AngularJS</t>
         </is>
       </c>
     </row>
@@ -1366,7 +1496,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Dưới 1 năm</t>
+          <t>1 năm</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1376,7 +1506,12 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Swift, Objective-C, Android</t>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>.NET, Laravel, VueJS, Bootstrap, FrontEnd</t>
         </is>
       </c>
     </row>
@@ -1401,7 +1536,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1 năm</t>
+          <t>2 năm</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1411,7 +1546,12 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>BackEnd, TypeScript, Flask, Sass/Less, NestJS</t>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>iOS, Kotlin, React Native, Android</t>
         </is>
       </c>
     </row>
@@ -1436,7 +1576,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1 năm</t>
+          <t>3 năm</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1446,7 +1586,12 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Android, Flutter, Objective-C, Kotlin, React Native</t>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Kiểm thử chức năng (Functional testing), Kiểm thử hiệu năng (Performance testing), Kiểm thử chấp nhận người dùng (User acceptance testing), Kiểm thử hệ thống (System testing), Kiểm thử tự động (Automation testing), Kiểm thử bảo mật (Security testing), Báo cáo kiểm thử (Test report)</t>
         </is>
       </c>
     </row>
@@ -1481,7 +1626,12 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Kiểm thử tải (Load testing), Kiểm thử tích hợp (Integration testing), Kiểm thử chấp nhận người dùng (User acceptance testing), Kiểm thử hệ thống (System testing), Báo cáo kiểm thử (Test report)</t>
+          <t>Tester/ QA/ QC</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>iOS, Swift, Objective-C, React Native, Kotlin</t>
         </is>
       </c>
     </row>
@@ -1506,7 +1656,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1 năm</t>
+          <t>Dưới 1 năm</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -1516,7 +1666,12 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Kiểm thử đơn vị (Unit testing), Kiểm thử hệ thống (System testing), Kiểm thử hồi quy (Regression testing), Kiểm thử tích hợp (Integration testing)</t>
+          <t>Tester/ QA/ QC</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>React Native, iOS, Swift</t>
         </is>
       </c>
     </row>
@@ -1541,7 +1696,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Dưới 1 năm</t>
+          <t>1 năm</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -1551,7 +1706,12 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Kiểm thử đơn vị (Unit testing), Kiểm thử chức năng (Functional testing), Kiểm thử hồi quy (Regression testing)</t>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>MongoDB, ReactJS, Python, NestJS, Laravel</t>
         </is>
       </c>
     </row>
@@ -1576,7 +1736,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1 năm</t>
+          <t>Dưới 1 năm</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -1586,7 +1746,12 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Objective-C, Swift, Android, Kotlin, Flutter</t>
+          <t>Mobile Developer</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Bootstrap, JavaScript, PHP</t>
         </is>
       </c>
     </row>
@@ -1621,7 +1786,12 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Objective-C, Android, Flutter, React Native, Kotlin, Swift</t>
+          <t>Tester/ QA/ QC</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Laravel, TypeScript, Django, PostgreSQL, NestJS, MySQL</t>
         </is>
       </c>
     </row>
@@ -1646,7 +1816,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1 năm</t>
+          <t>3 năm</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -1656,7 +1826,12 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Android, React Native, iOS, Flutter, Objective-C</t>
+          <t>Tester/ QA/ QC</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>React Native, Flutter, Swift, iOS, Kotlin</t>
         </is>
       </c>
     </row>
@@ -1691,7 +1866,12 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>jQuery, FrontEnd, NodeJS, JavaScript, VueJS</t>
+          <t>Tester/ QA/ QC</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>iOS, React Native, Objective-C, Swift</t>
         </is>
       </c>
     </row>
@@ -1716,7 +1896,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1 năm</t>
+          <t>3 năm</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -1726,7 +1906,12 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Git, MongoDB, Django, VueJS, Bootstrap</t>
+          <t>Tester/ QA/ QC</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>.NET, jQuery, Sass/Less, Python, NodeJS, BackEnd</t>
         </is>
       </c>
     </row>
@@ -1751,7 +1936,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>1 năm</t>
+          <t>2 năm</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -1761,7 +1946,12 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>React Native, Kotlin, Objective-C, Flutter</t>
+          <t>Tester/ QA/ QC</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Objective-C, React Native, Swift, Flutter</t>
         </is>
       </c>
     </row>
@@ -1786,7 +1976,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>1 năm</t>
+          <t>Dưới 1 năm</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -1796,7 +1986,12 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Python, Django, AngularJS, PostgreSQL</t>
+          <t>Mobile Developer</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>Kiểm thử hồi quy (Regression testing), Kiểm thử giao diện người dùng (User interface testing), Kiểm thử chấp nhận người dùng (User acceptance testing)</t>
         </is>
       </c>
     </row>
@@ -1831,7 +2026,12 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>React Native, Android, Kotlin, iOS, Swift, Objective-C</t>
+          <t>Mobile Developer</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>MySQL, Redis, Material UI, Flask, NestJS</t>
         </is>
       </c>
     </row>
@@ -1856,7 +2056,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>1 năm</t>
+          <t>2 năm</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -1866,7 +2066,12 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Kiểm thử bảo mật (Security testing), Kiểm thử chấp nhận người dùng (User acceptance testing), Báo cáo kiểm thử (Test report), Phân tích yêu cầu (Requirement analysis), Kiểm thử tự động (Automation testing)</t>
+          <t>Mobile Developer</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>Android, Kotlin, React Native, Flutter</t>
         </is>
       </c>
     </row>
@@ -1901,7 +2106,12 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Python, Spring Framework, Sass/Less, VueJS, Django, Material UI, TypeScript</t>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>Kiểm thử chấp nhận người dùng (User acceptance testing), Kiểm thử hệ thống (System testing), Báo cáo kiểm thử (Test report), Đặc tả kiểm thử (Test case specification), Kiểm thử tải (Load testing)</t>
         </is>
       </c>
     </row>
@@ -1926,7 +2136,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>3 năm</t>
+          <t>1 năm</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -1936,7 +2146,12 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Django, Material UI, Redis, PHP, .NET, NodeJS, MongoDB</t>
+          <t>Mobile Developer</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>Kotlin, Flutter, Android, React Native</t>
         </is>
       </c>
     </row>
@@ -1961,7 +2176,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Dưới 1 năm</t>
+          <t>2 năm</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -1971,7 +2186,12 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>React Native, iOS, Swift</t>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>Kotlin, React Native, Swift, Android</t>
         </is>
       </c>
     </row>
@@ -2006,7 +2226,12 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Phân tích yêu cầu (Requirement analysis), Kiểm thử tích hợp (Integration testing), Kiểm thử đơn vị (Unit testing), Kiểm thử bảo mật (Security testing), Đặc tả kiểm thử (Test case specification), Kiểm thử chấp nhận người dùng (User acceptance testing)</t>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>Kotlin, Flutter, React Native, Objective-C, iOS, Android, Swift</t>
         </is>
       </c>
     </row>
@@ -2031,7 +2256,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1 năm</t>
+          <t>Dưới 1 năm</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -2041,7 +2266,12 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Kiểm thử tích hợp (Integration testing), Kiểm thử giao diện người dùng (User interface testing), Kiểm thử hồi quy (Regression testing), Kiểm thử bảo mật (Security testing), Kiểm thử chức năng (Functional testing)</t>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>Laravel, PostgreSQL, NestJS</t>
         </is>
       </c>
     </row>
@@ -2076,7 +2306,12 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Spring Framework, BackEnd, MongoDB, NestJS, FrontEnd, Bootstrap</t>
+          <t>Tester/ QA/ QC</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>Kotlin, Swift, Android, Flutter, iOS, React Native, Objective-C</t>
         </is>
       </c>
     </row>
@@ -2101,7 +2336,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2 năm</t>
+          <t>Dưới 1 năm</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -2111,7 +2346,12 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>NestJS, Spring Framework, VueJS, .NET</t>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>PostgreSQL, MongoDB, Java</t>
         </is>
       </c>
     </row>
@@ -2136,7 +2376,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>3 năm</t>
+          <t>1 năm</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -2146,7 +2386,12 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Objective-C, Swift, Android, iOS, React Native, Flutter</t>
+          <t>Mobile Developer</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>Đặc tả kiểm thử (Test case specification), Kiểm thử bảo mật (Security testing), Phân tích yêu cầu (Requirement analysis), Kiểm thử tích hợp (Integration testing)</t>
         </is>
       </c>
     </row>
@@ -2181,7 +2426,12 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>React Native, Kotlin, Android, iOS, Objective-C, Swift</t>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>Django, Python, NestJS, Redis, NodeJS, Flask, Laravel</t>
         </is>
       </c>
     </row>
@@ -2206,7 +2456,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Dưới 1 năm</t>
+          <t>2 năm</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -2216,7 +2466,12 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>ReactJS, Material UI, Ruby on Rails</t>
+          <t>Tester/ QA/ QC</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>Kiểm thử hiệu năng (Performance testing), Kiểm thử giao diện người dùng (User interface testing), Phân tích yêu cầu (Requirement analysis), Báo cáo kiểm thử (Test report), Kiểm thử hệ thống (System testing)</t>
         </is>
       </c>
     </row>
@@ -2241,7 +2496,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>3 năm</t>
+          <t>2 năm</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -2251,7 +2506,12 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Kiểm thử đơn vị (Unit testing), Kiểm thử tự động (Automation testing), Kiểm thử tải (Load testing), Kiểm thử bảo mật (Security testing), Kiểm thử tích hợp (Integration testing), Kiểm thử hồi quy (Regression testing)</t>
+          <t>Tester/ QA/ QC</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>Phân tích yêu cầu (Requirement analysis), Kiểm thử tích hợp (Integration testing), Kiểm thử chấp nhận người dùng (User acceptance testing), Kiểm thử hiệu năng (Performance testing)</t>
         </is>
       </c>
     </row>
@@ -2276,7 +2536,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Dưới 1 năm</t>
+          <t>1 năm</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -2286,7 +2546,12 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>TypeScript, Laravel, NestJS</t>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>Kiểm thử tích hợp (Integration testing), Kiểm thử giao diện người dùng (User interface testing), Phân tích yêu cầu (Requirement analysis), Kiểm thử chức năng (Functional testing), Kiểm thử hiệu năng (Performance testing)</t>
         </is>
       </c>
     </row>
@@ -2321,7 +2586,12 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Kiểm thử tải (Load testing), Đặc tả kiểm thử (Test case specification), Kiểm thử hồi quy (Regression testing), Kiểm thử tích hợp (Integration testing), Kiểm thử tự động (Automation testing)</t>
+          <t>Tester/ QA/ QC</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>Kiểm thử tích hợp (Integration testing), Kiểm thử giao diện người dùng (User interface testing), Đặc tả kiểm thử (Test case specification), Kiểm thử tự động (Automation testing)</t>
         </is>
       </c>
     </row>
@@ -2356,7 +2626,12 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Redis, JavaScript, Laravel, PostgreSQL, MySQL</t>
+          <t>Tester/ QA/ QC</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>Flask, Ruby, Material UI, Sass/Less, Git, JavaScript, Python</t>
         </is>
       </c>
     </row>
@@ -2391,7 +2666,12 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Kiểm thử tích hợp (Integration testing), Báo cáo kiểm thử (Test report), Đặc tả kiểm thử (Test case specification)</t>
+          <t>Mobile Developer</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>Bootstrap, MySQL, PostgreSQL</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2706,12 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>Objective-C, React Native, Swift, Flutter, Kotlin, iOS</t>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>Material UI, JavaScript, Ruby on Rails, Bootstrap, NodeJS</t>
         </is>
       </c>
     </row>
@@ -2451,7 +2736,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>2 năm</t>
+          <t>1 năm</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -2461,7 +2746,12 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>MySQL, TypeScript, Bootstrap, ReactJS, VueJS</t>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>Báo cáo kiểm thử (Test report), Kiểm thử chấp nhận người dùng (User acceptance testing), Phân tích yêu cầu (Requirement analysis), Kiểm thử giao diện người dùng (User interface testing), Kiểm thử tải (Load testing)</t>
         </is>
       </c>
     </row>
@@ -2496,7 +2786,12 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>Phân tích yêu cầu (Requirement analysis), Kiểm thử hiệu năng (Performance testing), Báo cáo kiểm thử (Test report), Kiểm thử hệ thống (System testing)</t>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>Kiểm thử tải (Load testing), Đặc tả kiểm thử (Test case specification), Kiểm thử tự động (Automation testing), Phân tích yêu cầu (Requirement analysis), Kiểm thử chức năng (Functional testing)</t>
         </is>
       </c>
     </row>
@@ -2531,7 +2826,12 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>Kiểm thử giao diện người dùng (User interface testing), Kiểm thử đơn vị (Unit testing), Kiểm thử chức năng (Functional testing), Đặc tả kiểm thử (Test case specification), Kiểm thử hồi quy (Regression testing)</t>
+          <t>Mobile Developer</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>NestJS, BackEnd, ReactJS, Python, PHP, VueJS, FrontEnd</t>
         </is>
       </c>
     </row>
@@ -2556,7 +2856,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>3 năm</t>
+          <t>2 năm</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -2566,7 +2866,12 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>iOS, Objective-C, Swift, React Native, Flutter, Kotlin, Android</t>
+          <t>Tester/ QA/ QC</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>Kiểm thử đơn vị (Unit testing), Kiểm thử tải (Load testing), Kiểm thử tích hợp (Integration testing), Kiểm thử bảo mật (Security testing), Kiểm thử chấp nhận người dùng (User acceptance testing)</t>
         </is>
       </c>
     </row>
@@ -2591,7 +2896,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Dưới 1 năm</t>
+          <t>2 năm</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -2601,7 +2906,12 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>Phân tích yêu cầu (Requirement analysis), Báo cáo kiểm thử (Test report), Kiểm thử bảo mật (Security testing)</t>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>iOS, Objective-C, Android, Swift, Kotlin</t>
         </is>
       </c>
     </row>
@@ -2626,7 +2936,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>1 năm</t>
+          <t>2 năm</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -2636,7 +2946,12 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>Swift, Flutter, Android, iOS, React Native</t>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>Python, FrontEnd, Django, Bootstrap, Ruby on Rails</t>
         </is>
       </c>
     </row>
@@ -2661,7 +2976,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Dưới 1 năm</t>
+          <t>3 năm</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -2671,7 +2986,12 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>Objective-C, Android, Flutter</t>
+          <t>Mobile Developer</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>Kiểm thử bảo mật (Security testing), Kiểm thử đơn vị (Unit testing), Kiểm thử hiệu năng (Performance testing), Kiểm thử hệ thống (System testing), Phân tích yêu cầu (Requirement analysis)</t>
         </is>
       </c>
     </row>
@@ -2696,7 +3016,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>1 năm</t>
+          <t>3 năm</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -2706,7 +3026,12 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>iOS, Kotlin, Swift, React Native, Objective-C</t>
+          <t>Tester/ QA/ QC</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>Spring Framework, PostgreSQL, MySQL, Ruby, ReactJS, jQuery, NestJS</t>
         </is>
       </c>
     </row>
@@ -2731,7 +3056,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>3 năm</t>
+          <t>Dưới 1 năm</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -2741,7 +3066,12 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>Android, Swift, Objective-C, Kotlin, iOS</t>
+          <t>Mobile Developer</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>Swift, iOS, React Native</t>
         </is>
       </c>
     </row>
@@ -2766,7 +3096,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>2 năm</t>
+          <t>Dưới 1 năm</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -2776,7 +3106,12 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>Objective-C, iOS, React Native, Swift, Kotlin</t>
+          <t>Mobile Developer</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>Kotlin, Flutter, Objective-C</t>
         </is>
       </c>
     </row>
@@ -2801,7 +3136,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>2 năm</t>
+          <t>3 năm</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -2811,7 +3146,12 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>Python, jQuery, PHP, Git, Redis</t>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>Ruby on Rails, Bootstrap, ReactJS, Spring Framework, Material UI</t>
         </is>
       </c>
     </row>
@@ -2836,7 +3176,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>2 năm</t>
+          <t>Dưới 1 năm</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -2846,7 +3186,12 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>Kiểm thử chấp nhận người dùng (User acceptance testing), Báo cáo kiểm thử (Test report), Kiểm thử tự động (Automation testing), Phân tích yêu cầu (Requirement analysis)</t>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>.NET, Material UI, Flask</t>
         </is>
       </c>
     </row>
@@ -2871,7 +3216,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>2 năm</t>
+          <t>Dưới 1 năm</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -2881,7 +3226,12 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>Kotlin, React Native, iOS, Objective-C</t>
+          <t>Mobile Developer</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>MySQL, Java, Ruby</t>
         </is>
       </c>
     </row>
@@ -2906,7 +3256,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Dưới 1 năm</t>
+          <t>1 năm</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -2916,7 +3266,12 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>Kiểm thử bảo mật (Security testing), Kiểm thử giao diện người dùng (User interface testing), Báo cáo kiểm thử (Test report)</t>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>iOS, React Native, Objective-C, Swift</t>
         </is>
       </c>
     </row>
@@ -2941,7 +3296,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Dưới 1 năm</t>
+          <t>3 năm</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -2951,7 +3306,12 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>MySQL, Ruby, JavaScript</t>
+          <t>Mobile Developer</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>React Native, iOS, Objective-C, Kotlin, Flutter</t>
         </is>
       </c>
     </row>
@@ -2976,7 +3336,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>3 năm</t>
+          <t>1 năm</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -2986,7 +3346,12 @@
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>Flutter, Kotlin, iOS, Swift, React Native</t>
+          <t>Tester/ QA/ QC</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>Phân tích yêu cầu (Requirement analysis), Kiểm thử giao diện người dùng (User interface testing), Kiểm thử tự động (Automation testing), Kiểm thử hệ thống (System testing), Kiểm thử đơn vị (Unit testing)</t>
         </is>
       </c>
     </row>
@@ -3021,7 +3386,12 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>React Native, iOS, Android, Swift</t>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>ReactJS, AngularJS, Material UI, VueJS, Git</t>
         </is>
       </c>
     </row>
@@ -3046,7 +3416,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Dưới 1 năm</t>
+          <t>1 năm</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -3056,7 +3426,12 @@
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>Django, Sass/Less, PHP</t>
+          <t>Tester/ QA/ QC</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>jQuery, Laravel, VueJS, Sass/Less</t>
         </is>
       </c>
     </row>
@@ -3081,7 +3456,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>2 năm</t>
+          <t>1 năm</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -3091,7 +3466,12 @@
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>NestJS, jQuery, Bootstrap, TypeScript</t>
+          <t>Tester/ QA/ QC</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>PostgreSQL, Java, MongoDB, Django, .NET</t>
         </is>
       </c>
     </row>
@@ -3116,7 +3496,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>3 năm</t>
+          <t>2 năm</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -3126,7 +3506,12 @@
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>Kiểm thử chức năng (Functional testing), Phân tích yêu cầu (Requirement analysis), Đặc tả kiểm thử (Test case specification), Kiểm thử hiệu năng (Performance testing), Kiểm thử bảo mật (Security testing), Báo cáo kiểm thử (Test report), Kiểm thử hệ thống (System testing)</t>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>Kiểm thử giao diện người dùng (User interface testing), Kiểm thử hồi quy (Regression testing), Kiểm thử tự động (Automation testing), Phân tích yêu cầu (Requirement analysis)</t>
         </is>
       </c>
     </row>
@@ -3151,7 +3536,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>1 năm</t>
+          <t>3 năm</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -3161,7 +3546,12 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>Laravel, FrontEnd, ReactJS, Flask, PHP</t>
+          <t>Tester/ QA/ QC</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>NodeJS, Material UI, Ruby on Rails, VueJS, Flask, Django</t>
         </is>
       </c>
     </row>
@@ -3186,7 +3576,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Dưới 1 năm</t>
+          <t>2 năm</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -3196,7 +3586,12 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>Kiểm thử hiệu năng (Performance testing), Kiểm thử đơn vị (Unit testing), Báo cáo kiểm thử (Test report)</t>
+          <t>Mobile Developer</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>Objective-C, Kotlin, React Native, Flutter</t>
         </is>
       </c>
     </row>
@@ -3231,7 +3626,12 @@
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>Kiểm thử hệ thống (System testing), Kiểm thử hồi quy (Regression testing), Kiểm thử tải (Load testing), Kiểm thử đơn vị (Unit testing), Kiểm thử tích hợp (Integration testing)</t>
+          <t>Mobile Developer</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>Bootstrap, Laravel, PHP, VueJS, Sass/Less, Ruby, Spring Framework</t>
         </is>
       </c>
     </row>
@@ -3266,6 +3666,11 @@
       </c>
       <c r="G81" t="inlineStr">
         <is>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
           <t>React Native, Flutter, Swift</t>
         </is>
       </c>
@@ -3291,7 +3696,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>2 năm</t>
+          <t>1 năm</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -3301,7 +3706,12 @@
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>Kiểm thử tải (Load testing), Kiểm thử tích hợp (Integration testing), Kiểm thử chấp nhận người dùng (User acceptance testing), Kiểm thử hệ thống (System testing)</t>
+          <t>Mobile Developer</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>Kiểm thử tự động (Automation testing), Phân tích yêu cầu (Requirement analysis), Kiểm thử hiệu năng (Performance testing), Kiểm thử tải (Load testing)</t>
         </is>
       </c>
     </row>
@@ -3326,7 +3736,7 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>1 năm</t>
+          <t>Dưới 1 năm</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -3336,7 +3746,12 @@
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>Kiểm thử tự động (Automation testing), Kiểm thử tải (Load testing), Kiểm thử chấp nhận người dùng (User acceptance testing), Kiểm thử hồi quy (Regression testing)</t>
+          <t>Mobile Developer</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>NodeJS, JavaScript, VueJS</t>
         </is>
       </c>
     </row>
@@ -3361,7 +3776,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Dưới 1 năm</t>
+          <t>2 năm</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -3371,7 +3786,12 @@
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>Kiểm thử giao diện người dùng (User interface testing), Kiểm thử hồi quy (Regression testing), Kiểm thử hệ thống (System testing)</t>
+          <t>Mobile Developer</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>BackEnd, Flask, TypeScript, MongoDB, NodeJS</t>
         </is>
       </c>
     </row>
@@ -3396,7 +3816,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Dưới 1 năm</t>
+          <t>5 năm</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -3406,7 +3826,12 @@
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>Ruby, Java, Django</t>
+          <t>Mobile Developer</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>Kiểm thử hệ thống (System testing), Phân tích yêu cầu (Requirement analysis), Kiểm thử hiệu năng (Performance testing), Kiểm thử chức năng (Functional testing), Đặc tả kiểm thử (Test case specification), Kiểm thử giao diện người dùng (User interface testing), Kiểm thử tích hợp (Integration testing)</t>
         </is>
       </c>
     </row>
@@ -3431,7 +3856,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>3 năm</t>
+          <t>2 năm</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -3441,7 +3866,12 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>ReactJS, PostgreSQL, Django, jQuery, FrontEnd</t>
+          <t>Mobile Developer</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>.NET, PHP, Ruby, Laravel, Material UI</t>
         </is>
       </c>
     </row>
@@ -3466,7 +3896,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>1 năm</t>
+          <t>Chưa có kinh nghiệm</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -3476,7 +3906,12 @@
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>Swift, React Native, Objective-C, iOS, Flutter</t>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>Kiểm thử bảo mật (Security testing), Báo cáo kiểm thử (Test report), Kiểm thử đơn vị (Unit testing)</t>
         </is>
       </c>
     </row>
@@ -3501,7 +3936,7 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>1 năm</t>
+          <t>Dưới 1 năm</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -3511,7 +3946,12 @@
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>Flutter, React Native, Objective-C, Android</t>
+          <t>Tester/ QA/ QC</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>.NET, Django, NodeJS</t>
         </is>
       </c>
     </row>
@@ -3536,7 +3976,7 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>2 năm</t>
+          <t>Chưa có kinh nghiệm</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -3546,7 +3986,12 @@
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>iOS, Kotlin, Swift, Flutter, Android</t>
+          <t>Tester/ QA/ QC</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>Kiểm thử tích hợp (Integration testing), Đặc tả kiểm thử (Test case specification), Kiểm thử hệ thống (System testing)</t>
         </is>
       </c>
     </row>
@@ -3571,7 +4016,7 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>2 năm</t>
+          <t>Dưới 1 năm</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -3581,7 +4026,12 @@
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>Phân tích yêu cầu (Requirement analysis), Kiểm thử tự động (Automation testing), Kiểm thử tích hợp (Integration testing), Báo cáo kiểm thử (Test report), Kiểm thử đơn vị (Unit testing)</t>
+          <t>Tester/ QA/ QC</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>Bootstrap, NestJS, NodeJS</t>
         </is>
       </c>
     </row>
@@ -3606,7 +4056,7 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Dưới 1 năm</t>
+          <t>5 năm</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -3616,7 +4066,12 @@
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>Redis, TypeScript, BackEnd</t>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>AngularJS, MySQL, Ruby, ReactJS, PostgreSQL, Spring Framework, Sass/Less</t>
         </is>
       </c>
     </row>
@@ -3641,7 +4096,7 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Chưa có kinh nghiệm</t>
+          <t>Trên 5 năm</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -3651,7 +4106,12 @@
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>Git, NodeJS, ReactJS</t>
+          <t>Mobile Developer</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>Objective-C, Swift, Android, React Native, Flutter, Kotlin, iOS</t>
         </is>
       </c>
     </row>
@@ -3676,7 +4136,7 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Chưa có kinh nghiệm</t>
+          <t>4 năm</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -3686,7 +4146,12 @@
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>Kiểm thử tự động (Automation testing), Kiểm thử giao diện người dùng (User interface testing), Kiểm thử tích hợp (Integration testing)</t>
+          <t>Tester/ QA/ QC</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>Kiểm thử hồi quy (Regression testing), Kiểm thử đơn vị (Unit testing), Kiểm thử hiệu năng (Performance testing), Kiểm thử hệ thống (System testing), Kiểm thử tự động (Automation testing), Báo cáo kiểm thử (Test report)</t>
         </is>
       </c>
     </row>
@@ -3711,7 +4176,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>3 năm</t>
+          <t>Chưa có kinh nghiệm</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -3721,7 +4186,12 @@
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>NestJS, Git, AngularJS, PHP, FrontEnd</t>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>Java, NodeJS, Django</t>
         </is>
       </c>
     </row>
@@ -3746,7 +4216,7 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>2 năm</t>
+          <t>Dưới 1 năm</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -3756,7 +4226,12 @@
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>.NET, Flask, AngularJS, Ruby, Python</t>
+          <t>Mobile Developer</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>Kiểm thử bảo mật (Security testing), Kiểm thử chấp nhận người dùng (User acceptance testing), Kiểm thử giao diện người dùng (User interface testing)</t>
         </is>
       </c>
     </row>
@@ -3791,7 +4266,12 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>Django, Sass/Less, PHP, Bootstrap</t>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>Objective-C, Swift, React Native, Kotlin</t>
         </is>
       </c>
     </row>
@@ -3816,7 +4296,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>3 năm</t>
+          <t>Chưa có kinh nghiệm</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -3826,7 +4306,12 @@
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>NodeJS, NestJS, Material UI, AngularJS, Ruby on Rails</t>
+          <t>Tester/ QA/ QC</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>Flask, VueJS, Material UI</t>
         </is>
       </c>
     </row>
@@ -3851,7 +4336,7 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>4 năm</t>
+          <t>Dưới 1 năm</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
@@ -3861,7 +4346,12 @@
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>Java, Laravel, Git, jQuery, AngularJS, Bootstrap, MySQL</t>
+          <t>Mobile Developer</t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>Kiểm thử chấp nhận người dùng (User acceptance testing), Kiểm thử tự động (Automation testing), Báo cáo kiểm thử (Test report)</t>
         </is>
       </c>
     </row>
@@ -3886,7 +4376,7 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Chưa có kinh nghiệm</t>
+          <t>3 năm</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -3896,7 +4386,12 @@
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>TypeScript, BackEnd, MongoDB</t>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>Kiểm thử hệ thống (System testing), Kiểm thử đơn vị (Unit testing), Đặc tả kiểm thử (Test case specification), Báo cáo kiểm thử (Test report), Kiểm thử giao diện người dùng (User interface testing), Kiểm thử hồi quy (Regression testing), Kiểm thử chức năng (Functional testing)</t>
         </is>
       </c>
     </row>
@@ -3921,7 +4416,7 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>5 năm</t>
+          <t>3 năm</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -3931,7 +4426,12 @@
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>Objective-C, Android, iOS, Swift, Flutter, Kotlin</t>
+          <t>Tester/ QA/ QC</t>
+        </is>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>Laravel, Git, Python, Material UI, NestJS</t>
         </is>
       </c>
     </row>
@@ -3966,1757 +4466,12 @@
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>BackEnd, Java, AngularJS, MySQL</t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="n">
-        <v>101</v>
-      </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>Nguyễn Thành Hiền</t>
-        </is>
-      </c>
-      <c r="C102" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D102" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E102" t="inlineStr">
-        <is>
-          <t>5 năm</t>
-        </is>
-      </c>
-      <c r="F102" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G102" t="inlineStr">
-        <is>
-          <t>PostgreSQL, Sass/Less, NestJS, FrontEnd, ReactJS, Laravel</t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="n">
-        <v>102</v>
-      </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>Nguyễn Thành Hùng</t>
-        </is>
-      </c>
-      <c r="C103" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D103" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E103" t="inlineStr">
-        <is>
-          <t>Chưa có kinh nghiệm</t>
-        </is>
-      </c>
-      <c r="F103" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G103" t="inlineStr">
-        <is>
-          <t>VueJS, PHP, ReactJS</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="n">
-        <v>103</v>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>Nguyễn Thành Huy</t>
-        </is>
-      </c>
-      <c r="C104" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D104" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E104" t="inlineStr">
-        <is>
-          <t>1 năm</t>
-        </is>
-      </c>
-      <c r="F104" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G104" t="inlineStr">
-        <is>
-          <t>TypeScript, Sass/Less, PostgreSQL, JavaScript</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="n">
-        <v>104</v>
-      </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>Nguyễn Thành Khánh</t>
-        </is>
-      </c>
-      <c r="C105" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D105" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E105" t="inlineStr">
-        <is>
-          <t>3 năm</t>
-        </is>
-      </c>
-      <c r="F105" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G105" t="inlineStr">
-        <is>
-          <t>React Native, Objective-C, iOS, Kotlin, Android, Swift, Flutter</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="n">
-        <v>105</v>
-      </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>Nguyễn Thành Linh</t>
-        </is>
-      </c>
-      <c r="C106" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D106" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E106" t="inlineStr">
-        <is>
-          <t>5 năm</t>
-        </is>
-      </c>
-      <c r="F106" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G106" t="inlineStr">
-        <is>
-          <t>Objective-C, Android, Swift, Flutter, iOS</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="n">
-        <v>106</v>
-      </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>Nguyễn Thành Long</t>
-        </is>
-      </c>
-      <c r="C107" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D107" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E107" t="inlineStr">
-        <is>
-          <t>5 năm</t>
-        </is>
-      </c>
-      <c r="F107" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G107" t="inlineStr">
-        <is>
-          <t>iOS, Flutter, React Native, Kotlin, Android, Objective-C, Swift</t>
-        </is>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="n">
-        <v>107</v>
-      </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>Nguyễn Thành Nam</t>
-        </is>
-      </c>
-      <c r="C108" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D108" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E108" t="inlineStr">
-        <is>
-          <t>Chưa có kinh nghiệm</t>
-        </is>
-      </c>
-      <c r="F108" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G108" t="inlineStr">
-        <is>
-          <t>Kotlin, iOS, Android</t>
-        </is>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="n">
-        <v>108</v>
-      </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>Nguyễn Thành Nga</t>
-        </is>
-      </c>
-      <c r="C109" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D109" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E109" t="inlineStr">
-        <is>
-          <t>1 năm</t>
-        </is>
-      </c>
-      <c r="F109" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G109" t="inlineStr">
-        <is>
-          <t>Swift, Flutter, Android, Objective-C, Kotlin</t>
-        </is>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="n">
-        <v>109</v>
-      </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>Nguyễn Thành Nhi</t>
-        </is>
-      </c>
-      <c r="C110" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D110" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E110" t="inlineStr">
-        <is>
-          <t>3 năm</t>
-        </is>
-      </c>
-      <c r="F110" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G110" t="inlineStr">
-        <is>
-          <t>PHP, NestJS, Python, Sass/Less, Flask</t>
-        </is>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="n">
-        <v>110</v>
-      </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>Nguyễn Thành Phong</t>
-        </is>
-      </c>
-      <c r="C111" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D111" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E111" t="inlineStr">
-        <is>
-          <t>2 năm</t>
-        </is>
-      </c>
-      <c r="F111" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G111" t="inlineStr">
-        <is>
-          <t>Đặc tả kiểm thử (Test case specification), Kiểm thử tự động (Automation testing), Kiểm thử chức năng (Functional testing), Kiểm thử đơn vị (Unit testing)</t>
-        </is>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="n">
-        <v>111</v>
-      </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>Nguyễn Thành Phương</t>
-        </is>
-      </c>
-      <c r="C112" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D112" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E112" t="inlineStr">
-        <is>
-          <t>3 năm</t>
-        </is>
-      </c>
-      <c r="F112" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G112" t="inlineStr">
-        <is>
-          <t>Bootstrap, Django, Material UI, BackEnd, Sass/Less, FrontEnd, Java</t>
-        </is>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="n">
-        <v>112</v>
-      </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>Nguyễn Thành Quân</t>
-        </is>
-      </c>
-      <c r="C113" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D113" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E113" t="inlineStr">
-        <is>
-          <t>4 năm</t>
-        </is>
-      </c>
-      <c r="F113" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G113" t="inlineStr">
-        <is>
-          <t>Android, Flutter, iOS, Objective-C, React Native, Swift</t>
-        </is>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="n">
-        <v>113</v>
-      </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>Nguyễn Minh Anh</t>
-        </is>
-      </c>
-      <c r="C114" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D114" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E114" t="inlineStr">
-        <is>
-          <t>2 năm</t>
-        </is>
-      </c>
-      <c r="F114" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G114" t="inlineStr">
-        <is>
-          <t>Bootstrap, Redis, ReactJS, JavaScript, jQuery</t>
-        </is>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" t="n">
-        <v>114</v>
-      </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>Nguyễn Minh Bình</t>
-        </is>
-      </c>
-      <c r="C115" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D115" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E115" t="inlineStr">
-        <is>
-          <t>2 năm</t>
-        </is>
-      </c>
-      <c r="F115" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G115" t="inlineStr">
-        <is>
-          <t>TypeScript, PHP, Ruby on Rails, MySQL</t>
-        </is>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" t="n">
-        <v>115</v>
-      </c>
-      <c r="B116" t="inlineStr">
-        <is>
-          <t>Nguyễn Minh Cường</t>
-        </is>
-      </c>
-      <c r="C116" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D116" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E116" t="inlineStr">
-        <is>
-          <t>1 năm</t>
-        </is>
-      </c>
-      <c r="F116" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G116" t="inlineStr">
-        <is>
-          <t>Đặc tả kiểm thử (Test case specification), Kiểm thử tự động (Automation testing), Kiểm thử hồi quy (Regression testing), Kiểm thử hệ thống (System testing), Báo cáo kiểm thử (Test report)</t>
-        </is>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" t="n">
-        <v>116</v>
-      </c>
-      <c r="B117" t="inlineStr">
-        <is>
-          <t>Nguyễn Minh Dũng</t>
-        </is>
-      </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D117" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E117" t="inlineStr">
-        <is>
-          <t>Chưa có kinh nghiệm</t>
-        </is>
-      </c>
-      <c r="F117" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G117" t="inlineStr">
-        <is>
-          <t>Flutter, Objective-C, Android</t>
-        </is>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" t="n">
-        <v>117</v>
-      </c>
-      <c r="B118" t="inlineStr">
-        <is>
-          <t>Nguyễn Minh Hiền</t>
-        </is>
-      </c>
-      <c r="C118" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D118" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E118" t="inlineStr">
-        <is>
-          <t>2 năm</t>
-        </is>
-      </c>
-      <c r="F118" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G118" t="inlineStr">
-        <is>
-          <t>Kiểm thử giao diện người dùng (User interface testing), Báo cáo kiểm thử (Test report), Kiểm thử bảo mật (Security testing), Kiểm thử hồi quy (Regression testing), Kiểm thử hệ thống (System testing)</t>
-        </is>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" t="n">
-        <v>118</v>
-      </c>
-      <c r="B119" t="inlineStr">
-        <is>
-          <t>Nguyễn Minh Hùng</t>
-        </is>
-      </c>
-      <c r="C119" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D119" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E119" t="inlineStr">
-        <is>
-          <t>1 năm</t>
-        </is>
-      </c>
-      <c r="F119" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G119" t="inlineStr">
-        <is>
-          <t>Kiểm thử chức năng (Functional testing), Phân tích yêu cầu (Requirement analysis), Báo cáo kiểm thử (Test report), Kiểm thử hồi quy (Regression testing)</t>
-        </is>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" t="n">
-        <v>119</v>
-      </c>
-      <c r="B120" t="inlineStr">
-        <is>
-          <t>Nguyễn Minh Huy</t>
-        </is>
-      </c>
-      <c r="C120" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D120" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E120" t="inlineStr">
-        <is>
-          <t>Dưới 1 năm</t>
-        </is>
-      </c>
-      <c r="F120" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G120" t="inlineStr">
-        <is>
-          <t>Kiểm thử hiệu năng (Performance testing), Đặc tả kiểm thử (Test case specification), Kiểm thử tải (Load testing)</t>
-        </is>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" t="n">
-        <v>120</v>
-      </c>
-      <c r="B121" t="inlineStr">
-        <is>
-          <t>Nguyễn Minh Khánh</t>
-        </is>
-      </c>
-      <c r="C121" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D121" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E121" t="inlineStr">
-        <is>
-          <t>2 năm</t>
-        </is>
-      </c>
-      <c r="F121" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G121" t="inlineStr">
-        <is>
-          <t>Kiểm thử bảo mật (Security testing), Báo cáo kiểm thử (Test report), Đặc tả kiểm thử (Test case specification), Kiểm thử hệ thống (System testing), Kiểm thử tích hợp (Integration testing)</t>
-        </is>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" t="n">
-        <v>121</v>
-      </c>
-      <c r="B122" t="inlineStr">
-        <is>
-          <t>Nguyễn Minh Linh</t>
-        </is>
-      </c>
-      <c r="C122" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D122" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E122" t="inlineStr">
-        <is>
-          <t>2 năm</t>
-        </is>
-      </c>
-      <c r="F122" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G122" t="inlineStr">
-        <is>
-          <t>Báo cáo kiểm thử (Test report), Kiểm thử bảo mật (Security testing), Kiểm thử giao diện người dùng (User interface testing), Phân tích yêu cầu (Requirement analysis), Kiểm thử tích hợp (Integration testing)</t>
-        </is>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" t="n">
-        <v>122</v>
-      </c>
-      <c r="B123" t="inlineStr">
-        <is>
-          <t>Nguyễn Minh Long</t>
-        </is>
-      </c>
-      <c r="C123" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D123" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E123" t="inlineStr">
-        <is>
-          <t>Chưa có kinh nghiệm</t>
-        </is>
-      </c>
-      <c r="F123" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G123" t="inlineStr">
-        <is>
-          <t>jQuery, MongoDB, PHP</t>
-        </is>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" t="n">
-        <v>123</v>
-      </c>
-      <c r="B124" t="inlineStr">
-        <is>
-          <t>Nguyễn Minh Nam</t>
-        </is>
-      </c>
-      <c r="C124" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D124" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E124" t="inlineStr">
-        <is>
-          <t>3 năm</t>
-        </is>
-      </c>
-      <c r="F124" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G124" t="inlineStr">
-        <is>
-          <t>Spring Framework, ReactJS, Django, Sass/Less, NodeJS</t>
-        </is>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" t="n">
-        <v>124</v>
-      </c>
-      <c r="B125" t="inlineStr">
-        <is>
-          <t>Nguyễn Minh Nga</t>
-        </is>
-      </c>
-      <c r="C125" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D125" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E125" t="inlineStr">
-        <is>
-          <t>5 năm</t>
-        </is>
-      </c>
-      <c r="F125" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G125" t="inlineStr">
-        <is>
-          <t>Kiểm thử tự động (Automation testing), Kiểm thử hệ thống (System testing), Kiểm thử hiệu năng (Performance testing), Kiểm thử tải (Load testing), Kiểm thử đơn vị (Unit testing)</t>
-        </is>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" t="n">
-        <v>125</v>
-      </c>
-      <c r="B126" t="inlineStr">
-        <is>
-          <t>Nguyễn Minh Nhi</t>
-        </is>
-      </c>
-      <c r="C126" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D126" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E126" t="inlineStr">
-        <is>
-          <t>2 năm</t>
-        </is>
-      </c>
-      <c r="F126" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G126" t="inlineStr">
-        <is>
-          <t>Kotlin, iOS, Android, Objective-C, React Native</t>
-        </is>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" t="n">
-        <v>126</v>
-      </c>
-      <c r="B127" t="inlineStr">
-        <is>
-          <t>Nguyễn Minh Phong</t>
-        </is>
-      </c>
-      <c r="C127" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D127" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E127" t="inlineStr">
-        <is>
-          <t>Chưa có kinh nghiệm</t>
-        </is>
-      </c>
-      <c r="F127" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G127" t="inlineStr">
-        <is>
-          <t>Kiểm thử hồi quy (Regression testing), Báo cáo kiểm thử (Test report), Kiểm thử giao diện người dùng (User interface testing)</t>
-        </is>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" t="n">
-        <v>127</v>
-      </c>
-      <c r="B128" t="inlineStr">
-        <is>
-          <t>Nguyễn Minh Phương</t>
-        </is>
-      </c>
-      <c r="C128" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D128" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E128" t="inlineStr">
-        <is>
-          <t>5 năm</t>
-        </is>
-      </c>
-      <c r="F128" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G128" t="inlineStr">
-        <is>
-          <t>PHP, PostgreSQL, BackEnd, Spring Framework, NestJS, Laravel, Git</t>
-        </is>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" t="n">
-        <v>128</v>
-      </c>
-      <c r="B129" t="inlineStr">
-        <is>
-          <t>Nguyễn Minh Quân</t>
-        </is>
-      </c>
-      <c r="C129" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D129" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E129" t="inlineStr">
-        <is>
-          <t>Dưới 1 năm</t>
-        </is>
-      </c>
-      <c r="F129" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G129" t="inlineStr">
-        <is>
-          <t>Python, Material UI, Flask</t>
-        </is>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" t="n">
-        <v>129</v>
-      </c>
-      <c r="B130" t="inlineStr">
-        <is>
-          <t>Nguyễn Mạnh Anh</t>
-        </is>
-      </c>
-      <c r="C130" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D130" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E130" t="inlineStr">
-        <is>
-          <t>2 năm</t>
-        </is>
-      </c>
-      <c r="F130" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G130" t="inlineStr">
-        <is>
-          <t>Kiểm thử tự động (Automation testing), Kiểm thử tải (Load testing), Kiểm thử hồi quy (Regression testing), Kiểm thử tích hợp (Integration testing), Kiểm thử hệ thống (System testing)</t>
-        </is>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" t="n">
-        <v>130</v>
-      </c>
-      <c r="B131" t="inlineStr">
-        <is>
-          <t>Nguyễn Mạnh Bình</t>
-        </is>
-      </c>
-      <c r="C131" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D131" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E131" t="inlineStr">
-        <is>
-          <t>5 năm</t>
-        </is>
-      </c>
-      <c r="F131" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G131" t="inlineStr">
-        <is>
-          <t>Ruby, PostgreSQL, VueJS, Django, Python</t>
-        </is>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" t="n">
-        <v>131</v>
-      </c>
-      <c r="B132" t="inlineStr">
-        <is>
-          <t>Nguyễn Mạnh Cường</t>
-        </is>
-      </c>
-      <c r="C132" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D132" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E132" t="inlineStr">
-        <is>
-          <t>1 năm</t>
-        </is>
-      </c>
-      <c r="F132" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G132" t="inlineStr">
-        <is>
-          <t>MongoDB, ReactJS, PHP, PostgreSQL</t>
-        </is>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" t="n">
-        <v>132</v>
-      </c>
-      <c r="B133" t="inlineStr">
-        <is>
-          <t>Nguyễn Mạnh Dũng</t>
-        </is>
-      </c>
-      <c r="C133" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D133" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E133" t="inlineStr">
-        <is>
-          <t>5 năm</t>
-        </is>
-      </c>
-      <c r="F133" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G133" t="inlineStr">
-        <is>
-          <t>Sass/Less, VueJS, MySQL, Material UI, TypeScript</t>
-        </is>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" t="n">
-        <v>133</v>
-      </c>
-      <c r="B134" t="inlineStr">
-        <is>
-          <t>Nguyễn Mạnh Hiền</t>
-        </is>
-      </c>
-      <c r="C134" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D134" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E134" t="inlineStr">
-        <is>
-          <t>1 năm</t>
-        </is>
-      </c>
-      <c r="F134" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G134" t="inlineStr">
-        <is>
-          <t>iOS, React Native, Kotlin, Flutter, Swift</t>
-        </is>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135" t="n">
-        <v>134</v>
-      </c>
-      <c r="B135" t="inlineStr">
-        <is>
-          <t>Nguyễn Mạnh Hùng</t>
-        </is>
-      </c>
-      <c r="C135" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D135" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E135" t="inlineStr">
-        <is>
-          <t>Trên 5 năm</t>
-        </is>
-      </c>
-      <c r="F135" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G135" t="inlineStr">
-        <is>
-          <t>Python, AngularJS, Ruby, Sass/Less, ReactJS, Redis, Ruby on Rails</t>
-        </is>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136" t="n">
-        <v>135</v>
-      </c>
-      <c r="B136" t="inlineStr">
-        <is>
-          <t>Nguyễn Mạnh Huy</t>
-        </is>
-      </c>
-      <c r="C136" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D136" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E136" t="inlineStr">
-        <is>
-          <t>5 năm</t>
-        </is>
-      </c>
-      <c r="F136" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G136" t="inlineStr">
-        <is>
-          <t>Kotlin, Swift, Flutter, iOS, React Native</t>
-        </is>
-      </c>
-    </row>
-    <row r="137">
-      <c r="A137" t="n">
-        <v>136</v>
-      </c>
-      <c r="B137" t="inlineStr">
-        <is>
-          <t>Nguyễn Mạnh Khánh</t>
-        </is>
-      </c>
-      <c r="C137" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D137" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E137" t="inlineStr">
-        <is>
-          <t>2 năm</t>
-        </is>
-      </c>
-      <c r="F137" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G137" t="inlineStr">
-        <is>
-          <t>Flask, Bootstrap, .NET, BackEnd</t>
-        </is>
-      </c>
-    </row>
-    <row r="138">
-      <c r="A138" t="n">
-        <v>137</v>
-      </c>
-      <c r="B138" t="inlineStr">
-        <is>
-          <t>Nguyễn Mạnh Linh</t>
-        </is>
-      </c>
-      <c r="C138" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D138" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E138" t="inlineStr">
-        <is>
-          <t>Dưới 1 năm</t>
-        </is>
-      </c>
-      <c r="F138" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G138" t="inlineStr">
-        <is>
-          <t>React Native, iOS, Kotlin</t>
-        </is>
-      </c>
-    </row>
-    <row r="139">
-      <c r="A139" t="n">
-        <v>138</v>
-      </c>
-      <c r="B139" t="inlineStr">
-        <is>
-          <t>Nguyễn Mạnh Long</t>
-        </is>
-      </c>
-      <c r="C139" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D139" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E139" t="inlineStr">
-        <is>
-          <t>Chưa có kinh nghiệm</t>
-        </is>
-      </c>
-      <c r="F139" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G139" t="inlineStr">
-        <is>
-          <t>FrontEnd, NodeJS, AngularJS</t>
-        </is>
-      </c>
-    </row>
-    <row r="140">
-      <c r="A140" t="n">
-        <v>139</v>
-      </c>
-      <c r="B140" t="inlineStr">
-        <is>
-          <t>Nguyễn Mạnh Nam</t>
-        </is>
-      </c>
-      <c r="C140" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D140" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E140" t="inlineStr">
-        <is>
-          <t>4 năm</t>
-        </is>
-      </c>
-      <c r="F140" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G140" t="inlineStr">
-        <is>
-          <t>ReactJS, Bootstrap, NodeJS, Git, jQuery, PHP, TypeScript</t>
-        </is>
-      </c>
-    </row>
-    <row r="141">
-      <c r="A141" t="n">
-        <v>140</v>
-      </c>
-      <c r="B141" t="inlineStr">
-        <is>
-          <t>Nguyễn Mạnh Nga</t>
-        </is>
-      </c>
-      <c r="C141" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D141" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E141" t="inlineStr">
-        <is>
-          <t>Trên 5 năm</t>
-        </is>
-      </c>
-      <c r="F141" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G141" t="inlineStr">
-        <is>
-          <t>iOS, Kotlin, React Native, Objective-C, Flutter</t>
-        </is>
-      </c>
-    </row>
-    <row r="142">
-      <c r="A142" t="n">
-        <v>141</v>
-      </c>
-      <c r="B142" t="inlineStr">
-        <is>
-          <t>Nguyễn Mạnh Nhi</t>
-        </is>
-      </c>
-      <c r="C142" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D142" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E142" t="inlineStr">
-        <is>
-          <t>4 năm</t>
-        </is>
-      </c>
-      <c r="F142" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G142" t="inlineStr">
-        <is>
-          <t>Bootstrap, MySQL, Ruby, Spring Framework, Sass/Less</t>
-        </is>
-      </c>
-    </row>
-    <row r="143">
-      <c r="A143" t="n">
-        <v>142</v>
-      </c>
-      <c r="B143" t="inlineStr">
-        <is>
-          <t>Nguyễn Mạnh Phong</t>
-        </is>
-      </c>
-      <c r="C143" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D143" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E143" t="inlineStr">
-        <is>
-          <t>Chưa có kinh nghiệm</t>
-        </is>
-      </c>
-      <c r="F143" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G143" t="inlineStr">
-        <is>
-          <t>Swift, iOS, React Native</t>
-        </is>
-      </c>
-    </row>
-    <row r="144">
-      <c r="A144" t="n">
-        <v>143</v>
-      </c>
-      <c r="B144" t="inlineStr">
-        <is>
-          <t>Nguyễn Mạnh Phương</t>
-        </is>
-      </c>
-      <c r="C144" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D144" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E144" t="inlineStr">
-        <is>
-          <t>5 năm</t>
-        </is>
-      </c>
-      <c r="F144" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G144" t="inlineStr">
-        <is>
-          <t>iOS, Flutter, Android, Objective-C, React Native, Swift</t>
-        </is>
-      </c>
-    </row>
-    <row r="145">
-      <c r="A145" t="n">
-        <v>144</v>
-      </c>
-      <c r="B145" t="inlineStr">
-        <is>
-          <t>Nguyễn Mạnh Quân</t>
-        </is>
-      </c>
-      <c r="C145" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D145" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E145" t="inlineStr">
-        <is>
-          <t>3 năm</t>
-        </is>
-      </c>
-      <c r="F145" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G145" t="inlineStr">
-        <is>
-          <t>iOS, Android, Objective-C, Kotlin, Swift</t>
-        </is>
-      </c>
-    </row>
-    <row r="146">
-      <c r="A146" t="n">
-        <v>145</v>
-      </c>
-      <c r="B146" t="inlineStr">
-        <is>
-          <t>Nguyễn Văn Anh</t>
-        </is>
-      </c>
-      <c r="C146" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D146" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E146" t="inlineStr">
-        <is>
-          <t>Trên 5 năm</t>
-        </is>
-      </c>
-      <c r="F146" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G146" t="inlineStr">
-        <is>
-          <t>Kiểm thử đơn vị (Unit testing), Kiểm thử tích hợp (Integration testing), Kiểm thử hiệu năng (Performance testing), Kiểm thử chấp nhận người dùng (User acceptance testing), Kiểm thử tải (Load testing), Kiểm thử giao diện người dùng (User interface testing)</t>
-        </is>
-      </c>
-    </row>
-    <row r="147">
-      <c r="A147" t="n">
-        <v>146</v>
-      </c>
-      <c r="B147" t="inlineStr">
-        <is>
-          <t>Nguyễn Văn Bình</t>
-        </is>
-      </c>
-      <c r="C147" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D147" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E147" t="inlineStr">
-        <is>
-          <t>3 năm</t>
-        </is>
-      </c>
-      <c r="F147" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G147" t="inlineStr">
-        <is>
-          <t>iOS, Swift, Android, Flutter, Kotlin, React Native, Objective-C</t>
-        </is>
-      </c>
-    </row>
-    <row r="148">
-      <c r="A148" t="n">
-        <v>147</v>
-      </c>
-      <c r="B148" t="inlineStr">
-        <is>
-          <t>Nguyễn Văn Cường</t>
-        </is>
-      </c>
-      <c r="C148" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D148" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E148" t="inlineStr">
-        <is>
-          <t>3 năm</t>
-        </is>
-      </c>
-      <c r="F148" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G148" t="inlineStr">
-        <is>
-          <t>AngularJS, Spring Framework, NestJS, .NET, Sass/Less</t>
-        </is>
-      </c>
-    </row>
-    <row r="149">
-      <c r="A149" t="n">
-        <v>148</v>
-      </c>
-      <c r="B149" t="inlineStr">
-        <is>
-          <t>Nguyễn Văn Dũng</t>
-        </is>
-      </c>
-      <c r="C149" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D149" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E149" t="inlineStr">
-        <is>
-          <t>5 năm</t>
-        </is>
-      </c>
-      <c r="F149" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G149" t="inlineStr">
-        <is>
-          <t>React Native, Flutter, Swift, Kotlin, iOS</t>
-        </is>
-      </c>
-    </row>
-    <row r="150">
-      <c r="A150" t="n">
-        <v>149</v>
-      </c>
-      <c r="B150" t="inlineStr">
-        <is>
-          <t>Nguyễn Văn Hiền</t>
-        </is>
-      </c>
-      <c r="C150" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D150" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E150" t="inlineStr">
-        <is>
-          <t>1 năm</t>
-        </is>
-      </c>
-      <c r="F150" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G150" t="inlineStr">
-        <is>
-          <t>Android, iOS, React Native, Swift</t>
-        </is>
-      </c>
-    </row>
-    <row r="151">
-      <c r="A151" t="n">
-        <v>150</v>
-      </c>
-      <c r="B151" t="inlineStr">
-        <is>
-          <t>Nguyễn Văn Hùng</t>
-        </is>
-      </c>
-      <c r="C151" t="inlineStr">
-        <is>
-          <t>Hà Nội</t>
-        </is>
-      </c>
-      <c r="D151" t="inlineStr">
-        <is>
-          <t>Đại học</t>
-        </is>
-      </c>
-      <c r="E151" t="inlineStr">
-        <is>
-          <t>3 năm</t>
-        </is>
-      </c>
-      <c r="F151" t="inlineStr">
-        <is>
-          <t>Làm việc toàn thời gian</t>
-        </is>
-      </c>
-      <c r="G151" t="inlineStr">
-        <is>
-          <t>Kotlin, Objective-C, Android, Flutter, React Native, Swift</t>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>Kotlin, Objective-C, Swift, iOS, React Native</t>
         </is>
       </c>
     </row>

</xml_diff>